<commit_message>
Updates to diel activity code and results
</commit_message>
<xml_diff>
--- a/Example_data/Output/Predictions/MovementEcologyPaper/Supplementary_2_home_range_data.xlsx
+++ b/Example_data/Output/Predictions/MovementEcologyPaper/Supplementary_2_home_range_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s5236256\Documents\GitHub\ml4rt\Example_data\Output\Predictions\MovementEcologyPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C946D5B9-5B93-4F38-BFB2-3F619154ED81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951D6765-AEF5-4EF0-AAF4-E394DA62D2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="21120" windowHeight="11184" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -757,7 +757,7 @@
   <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>